<commit_message>
Se agrega campo isEmpy para contratos vacíos
</commit_message>
<xml_diff>
--- a/src/server/public/sources/plantilla.xlsx
+++ b/src/server/public/sources/plantilla.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
   <si>
     <t>C1</t>
   </si>
@@ -112,6 +112,9 @@
     <t>C33</t>
   </si>
   <si>
+    <t>C34</t>
+  </si>
+  <si>
     <t>Tipo de procedimiento</t>
   </si>
   <si>
@@ -209,6 +212,9 @@
   </si>
   <si>
     <t>Monto que excede el límite de la Adjudicación Directa</t>
+  </si>
+  <si>
+    <t>No se llevaron a cabo procedimientos</t>
   </si>
 </sst>
 </file>
@@ -261,7 +267,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -282,31 +288,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -318,7 +324,37 @@
         <color indexed="8"/>
       </right>
       <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -327,7 +363,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
@@ -340,36 +376,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -383,64 +389,64 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -460,10 +466,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff626868"/>
       <rgbColor rgb="ffdddddd"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -662,17 +668,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -700,10 +706,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -951,12 +957,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1243,7 +1249,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1271,10 +1277,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1525,42 +1531,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AG10"/>
+  <dimension ref="A1:AH10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.8125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.8516" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.8516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.9531" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" customWidth="1"/>
     <col min="4" max="7" width="10.8516" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.75" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.4688" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.6797" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5312" style="1" customWidth="1"/>
-    <col min="12" max="12" width="24.9844" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.2109" style="1" customWidth="1"/>
-    <col min="14" max="14" width="26.0781" style="1" customWidth="1"/>
-    <col min="15" max="15" width="23.9453" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.8516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.6719" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="25" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.1719" style="1" customWidth="1"/>
+    <col min="14" max="14" width="26.1719" style="1" customWidth="1"/>
+    <col min="15" max="15" width="24" style="1" customWidth="1"/>
     <col min="16" max="16" width="10.8516" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20.7656" style="1" customWidth="1"/>
-    <col min="18" max="18" width="21.1406" style="1" customWidth="1"/>
-    <col min="19" max="19" width="15.0938" style="1" customWidth="1"/>
-    <col min="20" max="20" width="18.8906" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.8516" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.1719" style="1" customWidth="1"/>
+    <col min="19" max="19" width="15.1719" style="1" customWidth="1"/>
+    <col min="20" max="20" width="18.8516" style="1" customWidth="1"/>
     <col min="21" max="21" width="10.8516" style="1" customWidth="1"/>
-    <col min="22" max="22" width="22.2734" style="1" customWidth="1"/>
+    <col min="22" max="22" width="22.3516" style="1" customWidth="1"/>
     <col min="23" max="23" width="13.1719" style="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5469" style="1" customWidth="1"/>
-    <col min="25" max="25" width="17.9609" style="1" customWidth="1"/>
-    <col min="26" max="26" width="22.9531" style="1" customWidth="1"/>
-    <col min="27" max="27" width="15.8672" style="1" customWidth="1"/>
-    <col min="28" max="28" width="13.1797" style="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5" style="1" customWidth="1"/>
+    <col min="25" max="25" width="18" style="1" customWidth="1"/>
+    <col min="26" max="26" width="23" style="1" customWidth="1"/>
+    <col min="27" max="27" width="15.8516" style="1" customWidth="1"/>
+    <col min="28" max="28" width="13.1719" style="1" customWidth="1"/>
     <col min="29" max="30" width="10.8516" style="1" customWidth="1"/>
-    <col min="31" max="31" width="18.1328" style="1" customWidth="1"/>
-    <col min="32" max="32" width="22.6016" style="1" customWidth="1"/>
-    <col min="33" max="33" width="23.6953" style="1" customWidth="1"/>
-    <col min="34" max="256" width="10.8516" style="1" customWidth="1"/>
+    <col min="31" max="31" width="18.1719" style="1" customWidth="1"/>
+    <col min="32" max="32" width="22.6719" style="1" customWidth="1"/>
+    <col min="33" max="34" width="23.6719" style="1" customWidth="1"/>
+    <col min="35" max="256" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
@@ -1663,106 +1669,112 @@
       <c r="AG1" t="s" s="2">
         <v>32</v>
       </c>
+      <c r="AH1" t="s" s="2">
+        <v>33</v>
+      </c>
     </row>
     <row r="2" ht="50" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s" s="4">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H2" t="s" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I2" t="s" s="4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J2" t="s" s="4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K2" t="s" s="4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s" s="4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M2" t="s" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N2" t="s" s="4">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O2" t="s" s="4">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P2" t="s" s="4">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q2" t="s" s="4">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R2" t="s" s="4">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S2" t="s" s="4">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="T2" t="s" s="4">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="U2" t="s" s="4">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="V2" t="s" s="4">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="W2" t="s" s="4">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="X2" t="s" s="4">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Y2" t="s" s="4">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Z2" t="s" s="4">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AA2" t="s" s="4">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AB2" t="s" s="4">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AC2" t="s" s="4">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD2" t="s" s="4">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AE2" t="s" s="4">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AF2" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="AG2" t="s" s="5">
         <v>65</v>
+      </c>
+      <c r="AG2" t="s" s="4">
+        <v>66</v>
+      </c>
+      <c r="AH2" t="s" s="5">
+        <v>67</v>
       </c>
     </row>
     <row r="3" ht="17" customHeight="1">
@@ -1799,6 +1811,7 @@
       <c r="AE3" s="11"/>
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
     </row>
     <row r="4" ht="17" customHeight="1">
       <c r="A4" s="12"/>
@@ -1834,6 +1847,7 @@
       <c r="AE4" s="18"/>
       <c r="AF4" s="12"/>
       <c r="AG4" s="12"/>
+      <c r="AH4" s="12"/>
     </row>
     <row r="5" ht="17" customHeight="1">
       <c r="A5" s="12"/>
@@ -1869,6 +1883,7 @@
       <c r="AE5" s="18"/>
       <c r="AF5" s="12"/>
       <c r="AG5" s="12"/>
+      <c r="AH5" s="12"/>
     </row>
     <row r="6" ht="17" customHeight="1">
       <c r="A6" s="12"/>
@@ -1904,6 +1919,7 @@
       <c r="AE6" s="12"/>
       <c r="AF6" s="12"/>
       <c r="AG6" s="12"/>
+      <c r="AH6" s="12"/>
     </row>
     <row r="7" ht="17" customHeight="1">
       <c r="A7" s="12"/>
@@ -1939,6 +1955,7 @@
       <c r="AE7" s="12"/>
       <c r="AF7" s="12"/>
       <c r="AG7" s="12"/>
+      <c r="AH7" s="12"/>
     </row>
     <row r="8" ht="17" customHeight="1">
       <c r="A8" s="12"/>
@@ -1974,6 +1991,7 @@
       <c r="AE8" s="12"/>
       <c r="AF8" s="12"/>
       <c r="AG8" s="12"/>
+      <c r="AH8" s="12"/>
     </row>
     <row r="9" ht="17" customHeight="1">
       <c r="A9" s="12"/>
@@ -2009,6 +2027,7 @@
       <c r="AE9" s="12"/>
       <c r="AF9" s="12"/>
       <c r="AG9" s="12"/>
+      <c r="AH9" s="12"/>
     </row>
     <row r="10" ht="17" customHeight="1">
       <c r="A10" s="12"/>
@@ -2044,6 +2063,7 @@
       <c r="AE10" s="12"/>
       <c r="AF10" s="12"/>
       <c r="AG10" s="12"/>
+      <c r="AH10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>